<commit_message>
optimisation supplémentaire et fin de la documentation de l'extension
</commit_message>
<xml_diff>
--- a/docs/optimisation/benchmark.xlsx
+++ b/docs/optimisation/benchmark.xlsx
@@ -988,7 +988,12 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:x val="0.010460000000000001"/>
+          <c:y val="-0.01048"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr bwMode="auto">
         <a:prstGeom prst="rect">
@@ -1613,7 +1618,7 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="2514599" y="8334373"/>
+      <a:off x="2514599" y="8524873"/>
       <a:ext cx="4552949" cy="2724149"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
@@ -2812,14 +2817,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>9523</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>19048</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>19048</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>28573</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2829,7 +2834,7 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2514599" y="8334373"/>
+        <a:off x="2514599" y="8524873"/>
         <a:ext cx="4552949" cy="2724149"/>
       </xdr:xfrm>
       <a:graphic>

</xml_diff>